<commit_message>
Added enum and budget
Next: add test
</commit_message>
<xml_diff>
--- a/restful/tst/dummy_data.xlsx
+++ b/restful/tst/dummy_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zijie/IDE_Projects/python/home-dashboard-backend/restful/tst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C12215-3C2B-BF4C-9EA8-48A60A5FE42E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477C7D47-3260-344A-A374-A47A1EA5FB15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17440" yWindow="10720" windowWidth="16160" windowHeight="10280" xr2:uid="{B6CC2591-C8D6-5240-9A07-519CBDD1F61A}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>icon</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>time_created</t>
   </si>
   <si>
-    <t>test icon 1</t>
-  </si>
-  <si>
     <t>Food</t>
   </si>
   <si>
@@ -75,9 +69,6 @@
     <t>2020 3 25 18 00 00</t>
   </si>
   <si>
-    <t>test icon 2</t>
-  </si>
-  <si>
     <t>Toy</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t>Index VR</t>
   </si>
   <si>
-    <t>test icon 3</t>
-  </si>
-  <si>
     <t>Stock</t>
   </si>
   <si>
@@ -100,9 +88,6 @@
   </si>
   <si>
     <t>Stock income</t>
-  </si>
-  <si>
-    <t>test icon 4</t>
   </si>
   <si>
     <t>2020 2 24 19 00 10</t>
@@ -177,8 +162,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,208 +481,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A3DD2E3-9179-7649-AFB8-0627AFFA3E4C}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>-12</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-1099</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
-        <v>-1099</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-21.5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-5.19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>711</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-4</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>-21.5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7000</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>-5.19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6">
-        <v>711</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>-4</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>7000</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>